<commit_message>
make sure all nodes have correct number of children
</commit_message>
<xml_diff>
--- a/OrgHier.xlsx
+++ b/OrgHier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -28,52 +28,88 @@
     <t>SALES</t>
   </si>
   <si>
-    <t>Pam.Suckow6</t>
-  </si>
-  <si>
-    <t>Pam Suckow</t>
-  </si>
-  <si>
-    <t>Paulita.Fassino2</t>
-  </si>
-  <si>
-    <t>Vincenzo.Pasch2</t>
-  </si>
-  <si>
-    <t>Vincenzo Pasch</t>
-  </si>
-  <si>
-    <t>Kary.Brasil0</t>
-  </si>
-  <si>
-    <t>Kary Brasil</t>
-  </si>
-  <si>
-    <t>Paulita Fassino</t>
-  </si>
-  <si>
-    <t>Jake.Asbell9</t>
-  </si>
-  <si>
-    <t>Jake Asbell</t>
-  </si>
-  <si>
-    <t>Francesco.Sandstrom4</t>
-  </si>
-  <si>
-    <t>Kristine.Lehr1</t>
-  </si>
-  <si>
-    <t>Kristine Lehr</t>
-  </si>
-  <si>
-    <t>Ivy.Palas7</t>
-  </si>
-  <si>
-    <t>Ivy Palas</t>
-  </si>
-  <si>
-    <t>Francesco Sandstrom</t>
+    <t>Ruben.Pruyn2</t>
+  </si>
+  <si>
+    <t>Ruben Pruyn</t>
+  </si>
+  <si>
+    <t>Maira.Roberts3</t>
+  </si>
+  <si>
+    <t>Olene.Markiewicz1</t>
+  </si>
+  <si>
+    <t>Olene Markiewicz</t>
+  </si>
+  <si>
+    <t>Kyra.Verra0</t>
+  </si>
+  <si>
+    <t>Kyra Verra</t>
+  </si>
+  <si>
+    <t>Maira Roberts</t>
+  </si>
+  <si>
+    <t>Lorna.Hasbell7</t>
+  </si>
+  <si>
+    <t>Lorna Hasbell</t>
+  </si>
+  <si>
+    <t>Kimbra.Agnew4</t>
+  </si>
+  <si>
+    <t>Nola.Terstage0</t>
+  </si>
+  <si>
+    <t>Nola Terstage</t>
+  </si>
+  <si>
+    <t>Earnest.Gwynn5</t>
+  </si>
+  <si>
+    <t>Earnest Gwynn</t>
+  </si>
+  <si>
+    <t>Kimbra Agnew</t>
+  </si>
+  <si>
+    <t>Dede.Waligora9</t>
+  </si>
+  <si>
+    <t>Dede Waligora</t>
+  </si>
+  <si>
+    <t>Gaynell.Toyota1</t>
+  </si>
+  <si>
+    <t>Gaynell Toyota</t>
+  </si>
+  <si>
+    <t>Pamela.Harvilla6</t>
+  </si>
+  <si>
+    <t>Pamela Harvilla</t>
+  </si>
+  <si>
+    <t>Deadra.Ciullo5</t>
+  </si>
+  <si>
+    <t>Deadra Ciullo</t>
+  </si>
+  <si>
+    <t>Corrinne.Pesch6</t>
+  </si>
+  <si>
+    <t>Corrinne Pesch</t>
+  </si>
+  <si>
+    <t>Michaele.Trucks6</t>
+  </si>
+  <si>
+    <t>Michaele Trucks</t>
   </si>
 </sst>
 </file>
@@ -405,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -436,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -450,7 +486,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -464,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -475,7 +511,7 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -489,7 +525,7 @@
         <v>14</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -503,7 +539,7 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -517,7 +553,7 @@
         <v>14</v>
       </c>
       <c r="D8">
-        <v>94</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -528,7 +564,91 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>33</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed incorrect child being created during level creation due to for loop syntax incorrect
</commit_message>
<xml_diff>
--- a/OrgHier.xlsx
+++ b/OrgHier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -28,10 +28,100 @@
     <t>SALES</t>
   </si>
   <si>
-    <t>Joycelyn.Bovio-c3c00bc0</t>
-  </si>
-  <si>
-    <t>Joycelyn Bovio</t>
+    <t>Lanita.Kamradt-bda2a6fb</t>
+  </si>
+  <si>
+    <t>Lanita Kamradt</t>
+  </si>
+  <si>
+    <t>Leisa.Tatom-3971dd4d</t>
+  </si>
+  <si>
+    <t>Bettyann.Dimitt-5808fb09</t>
+  </si>
+  <si>
+    <t>Bettyann Dimitt</t>
+  </si>
+  <si>
+    <t>Oralia.Gaekle-77943eed</t>
+  </si>
+  <si>
+    <t>Oralia Gaekle</t>
+  </si>
+  <si>
+    <t>Ruben.Busman-0abbd40f</t>
+  </si>
+  <si>
+    <t>Ruben Busman</t>
+  </si>
+  <si>
+    <t>Bernetta.Shaske-120785f5</t>
+  </si>
+  <si>
+    <t>Bernetta Shaske</t>
+  </si>
+  <si>
+    <t>Leisa Tatom</t>
+  </si>
+  <si>
+    <t>Renee.Limerick-400a4c02</t>
+  </si>
+  <si>
+    <t>Renee Limerick</t>
+  </si>
+  <si>
+    <t>Deon.Simcoe-54054eb7</t>
+  </si>
+  <si>
+    <t>Deon Simcoe</t>
+  </si>
+  <si>
+    <t>Samuel.Zatarain-1f4e7caa</t>
+  </si>
+  <si>
+    <t>Samuel Zatarain</t>
+  </si>
+  <si>
+    <t>Rosaura.Pajtas-258b3c40</t>
+  </si>
+  <si>
+    <t>Rosaura Pajtas</t>
+  </si>
+  <si>
+    <t>Phyllis.Macabeo-09608125</t>
+  </si>
+  <si>
+    <t>Phyllis Macabeo</t>
+  </si>
+  <si>
+    <t>Ruthann.Cruthird-48a47c00</t>
+  </si>
+  <si>
+    <t>Ruthann Cruthird</t>
+  </si>
+  <si>
+    <t>Venus.Viau-58f152ff</t>
+  </si>
+  <si>
+    <t>Venus Viau</t>
+  </si>
+  <si>
+    <t>Rosia.Dobler-ea457b1c</t>
+  </si>
+  <si>
+    <t>Rosia Dobler</t>
+  </si>
+  <si>
+    <t>Mila.Ballinger-53aa6286</t>
+  </si>
+  <si>
+    <t>Mila Ballinger</t>
+  </si>
+  <si>
+    <t>Marylou.Merrit-9744b125</t>
+  </si>
+  <si>
+    <t>Marylou Merrit</t>
   </si>
 </sst>
 </file>
@@ -363,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,8 +480,218 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
       <c r="D2">
-        <v>38</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>